<commit_message>
Commit Auto (Tue Jul  9 17:53:31     2024)
</commit_message>
<xml_diff>
--- a/INFO/IceGroup (Категорий) (111).xlsx
+++ b/INFO/IceGroup (Категорий) (111).xlsx
@@ -7,19 +7,20 @@
     <workbookView xWindow="17625" yWindow="2190" windowWidth="10635" windowHeight="10335" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PRODUCTS" sheetId="7" r:id="rId1"/>
-    <sheet name="Холодильные шкафы" sheetId="6" r:id="rId2"/>
-    <sheet name="Морозильники" sheetId="3" r:id="rId3"/>
-    <sheet name="Камеры" sheetId="4" r:id="rId4"/>
-    <sheet name="Ларь" sheetId="2" r:id="rId5"/>
-    <sheet name="Бонеты" sheetId="1" r:id="rId6"/>
+    <sheet name="Холодильные витрины" sheetId="8" r:id="rId1"/>
+    <sheet name="Морозильники" sheetId="3" r:id="rId2"/>
+    <sheet name="PRODUCTS" sheetId="7" r:id="rId3"/>
+    <sheet name="Холодильные шкафы" sheetId="6" r:id="rId4"/>
+    <sheet name="Камеры" sheetId="4" r:id="rId5"/>
+    <sheet name="Ларь" sheetId="2" r:id="rId6"/>
+    <sheet name="Бонеты" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="260">
   <si>
     <t>Title</t>
   </si>
@@ -478,15 +479,6 @@
   </si>
   <si>
     <t>Морозильник для мороженого</t>
-  </si>
-  <si>
-    <t>морозильник +для мороженого</t>
-  </si>
-  <si>
-    <t>морозильная витрина +для мороженого</t>
-  </si>
-  <si>
-    <t>купить морозильник +для мороженого</t>
   </si>
   <si>
     <t>Холодильные шкафы</t>
@@ -2688,6 +2680,432 @@
   <si>
     <t>Холодильная камера 
 ДОБАВЛЮ + все товары с глухими дверьми</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Морозильники для магазина - торговые морозильные и холодильные решения</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Морозильные и холодильные лари
+Морозильная и холодильная бонета
+Морозильные шкафы для общепита
+Морозильные витрины для магазина
+Морозильная витрина для мороженого</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Морозильная камера
+Промышленный морозильник</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Преимущества промышленных морозильных камер</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Использование морозильных камер предоставляет множество преимуществ для бизнеса
+Применение морозильных камер в различных отраслях
+Типы морозильных камер
+Выбор морозильных камер для бизнеса
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Морозильные витрины</t>
+  </si>
+  <si>
+    <t>Бонеты</t>
+  </si>
+  <si>
+    <t>Холодильные витрины</t>
+  </si>
+  <si>
+    <t>Холодильные витрины Carboma</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Кондитерские витрины</t>
+  </si>
+  <si>
+    <t>Тепловая витрина</t>
+  </si>
+  <si>
+    <t>Открытые витрины</t>
+  </si>
+  <si>
+    <t>Настольная витрина</t>
+  </si>
+  <si>
+    <t>Камеры (старая стр)</t>
+  </si>
+  <si>
+    <t>Холодильники (старая стр Холодильные шкафы)</t>
+  </si>
+  <si>
+    <t>Горки (старая стр)</t>
   </si>
 </sst>
 </file>
@@ -3227,7 +3645,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3387,6 +3805,15 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3694,12 +4121,325 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="9" tint="-0.249977111117893"/>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="149.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18">
+      <c r="A2" s="73"/>
+      <c r="B2" s="39" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="65"/>
+      <c r="D2" s="72"/>
+    </row>
+    <row r="3" spans="1:4" ht="76.5">
+      <c r="A3" s="73"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" s="58"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="74"/>
+    </row>
+    <row r="5" spans="1:4" ht="18">
+      <c r="A5" s="73">
+        <v>1</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" s="65"/>
+      <c r="D5" s="72"/>
+    </row>
+    <row r="6" spans="1:4" ht="91.5">
+      <c r="A6" s="73"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="57" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" s="58"/>
+    </row>
+    <row r="7" spans="1:4" ht="18.75">
+      <c r="A7" s="74"/>
+      <c r="B7" s="32"/>
+    </row>
+    <row r="8" spans="1:4" ht="18">
+      <c r="A8" s="73">
+        <v>2</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" s="65"/>
+      <c r="D8" s="72"/>
+    </row>
+    <row r="9" spans="1:4" ht="76.5">
+      <c r="A9" s="73"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="58"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="74"/>
+    </row>
+    <row r="11" spans="1:4" ht="18">
+      <c r="A11" s="73">
+        <v>3</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="65"/>
+      <c r="D11" s="72"/>
+    </row>
+    <row r="12" spans="1:4" ht="76.5">
+      <c r="A12" s="73"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12" s="58"/>
+    </row>
+    <row r="14" spans="1:4" ht="18">
+      <c r="A14" s="73">
+        <v>4</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="65"/>
+      <c r="D14" s="72"/>
+    </row>
+    <row r="15" spans="1:4" ht="76.5">
+      <c r="A15" s="73"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" s="58"/>
+    </row>
+    <row r="17" spans="1:4" ht="18">
+      <c r="A17" s="73">
+        <v>5</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="C17" s="65"/>
+      <c r="D17" s="72"/>
+    </row>
+    <row r="18" spans="1:4" ht="76.5">
+      <c r="A18" s="73"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D18" s="58"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="B20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="B21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="B22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D12" sqref="A1:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" style="74" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="119.7109375" customWidth="1"/>
+    <col min="4" max="4" width="160.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18">
+      <c r="A2" s="73"/>
+      <c r="B2" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="166.5">
+      <c r="A3" s="73"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="57" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="58"/>
+    </row>
+    <row r="5" spans="1:4" ht="18">
+      <c r="A5" s="73">
+        <v>1</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="72" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="136.5">
+      <c r="A6" s="73"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="57" t="s">
+        <v>247</v>
+      </c>
+      <c r="D6" s="58"/>
+    </row>
+    <row r="7" spans="1:4" ht="18.75">
+      <c r="B7" s="32"/>
+    </row>
+    <row r="8" spans="1:4" ht="18">
+      <c r="A8" s="73">
+        <v>2</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="65"/>
+      <c r="D8" s="72"/>
+    </row>
+    <row r="9" spans="1:4" ht="76.5">
+      <c r="A9" s="73"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="58"/>
+    </row>
+    <row r="11" spans="1:4" ht="18">
+      <c r="A11" s="73">
+        <v>3</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="65"/>
+      <c r="D11" s="72"/>
+    </row>
+    <row r="12" spans="1:4" ht="76.5">
+      <c r="A12" s="73"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="57" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12" s="58"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="74">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="74">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="74">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3713,14 +4453,14 @@
     <row r="1" spans="2:4" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:4" ht="15.75" thickBot="1">
       <c r="B2" s="52" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="48"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1">
       <c r="B3" s="49" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C3" s="50" t="s">
         <v>0</v>
@@ -3731,40 +4471,40 @@
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="59" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C4" s="60" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="141" thickBot="1">
       <c r="B5" s="62" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C5" s="63"/>
       <c r="D5" s="64"/>
     </row>
     <row r="7" spans="2:4">
       <c r="C7" s="53" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="C8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="C10" s="53" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="60">
       <c r="C11" s="54" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D11" s="54"/>
     </row>
@@ -3777,12 +4517,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3798,7 +4541,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
@@ -3810,22 +4553,22 @@
     <row r="2" spans="1:4" ht="18">
       <c r="A2" s="35"/>
       <c r="B2" s="39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C2" s="65" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D2" s="65" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="156" customHeight="1">
       <c r="A3" s="35"/>
       <c r="B3" s="41" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D3" s="58"/>
     </row>
@@ -3838,22 +4581,22 @@
         <v>1</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D5" s="56" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="169.5" customHeight="1">
       <c r="A6" s="35"/>
       <c r="B6" s="42" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C6" s="57" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D6" s="58"/>
     </row>
@@ -3866,22 +4609,22 @@
         <v>2</v>
       </c>
       <c r="B8" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="56" t="s">
         <v>178</v>
-      </c>
-      <c r="C8" s="66" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8" s="56" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="168">
       <c r="A9" s="35"/>
       <c r="B9" s="42" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D9" s="58"/>
     </row>
@@ -3894,22 +4637,22 @@
         <v>3</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C11" s="56" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D11" s="66" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="155.25" customHeight="1">
       <c r="A12" s="35"/>
       <c r="B12" s="42" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D12" s="58"/>
     </row>
@@ -3922,22 +4665,22 @@
         <v>4</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C14" s="66" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D14" s="66" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="149.25" customHeight="1">
       <c r="A15" s="35"/>
       <c r="B15" s="41" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C15" s="67" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D15" s="58"/>
     </row>
@@ -3949,25 +4692,25 @@
         <v>5</v>
       </c>
       <c r="B17" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" s="68" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" s="69" t="s">
         <v>190</v>
-      </c>
-      <c r="C17" s="68" t="s">
-        <v>192</v>
-      </c>
-      <c r="D17" s="69" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="133.5" customHeight="1">
       <c r="A18" s="35"/>
       <c r="B18" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="67" t="s">
         <v>191</v>
       </c>
-      <c r="C18" s="67" t="s">
-        <v>194</v>
-      </c>
       <c r="D18" s="70" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3978,22 +4721,22 @@
         <v>6</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C20" s="66" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D20" s="66" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="133.5" customHeight="1">
       <c r="A21" s="35"/>
       <c r="B21" s="42" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C21" s="67" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D21" s="58"/>
     </row>
@@ -4005,22 +4748,22 @@
         <v>7</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D23" s="56" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="119.25" customHeight="1">
       <c r="A24" s="35"/>
       <c r="B24" s="41" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C24" s="67" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D24" s="58"/>
     </row>
@@ -4032,22 +4775,22 @@
         <v>8</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C26" s="56" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D26" s="56" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="232.5" customHeight="1">
       <c r="A27" s="35"/>
       <c r="B27" s="42" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C27" s="67" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D27" s="58"/>
     </row>
@@ -4059,22 +4802,22 @@
         <v>9</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C29" s="56" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D29" s="56" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="149.25" customHeight="1">
       <c r="A30" s="35"/>
       <c r="B30" s="46" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C30" s="67" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D30" s="58"/>
     </row>
@@ -4084,22 +4827,22 @@
     <row r="32" spans="1:4" ht="18.75">
       <c r="A32" s="35"/>
       <c r="B32" s="40" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D32" s="66" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="141" customHeight="1">
       <c r="A33" s="35"/>
       <c r="B33" s="41" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C33" s="67" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D33" s="58"/>
     </row>
@@ -4109,22 +4852,22 @@
     <row r="35" spans="1:4" ht="18.75">
       <c r="A35" s="35"/>
       <c r="B35" s="40" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C35" s="56" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D35" s="56" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="125.25" customHeight="1">
       <c r="A36" s="35"/>
       <c r="B36" s="55" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C36" s="67" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D36" s="58"/>
     </row>
@@ -4134,25 +4877,25 @@
     <row r="38" spans="1:4" ht="18.75">
       <c r="A38" s="35"/>
       <c r="B38" s="40" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C38" s="66" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D38" s="66" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="114" customHeight="1">
       <c r="A39" s="35"/>
       <c r="B39" s="42" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C39" s="67" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D39" s="71" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -4160,21 +4903,21 @@
     </row>
     <row r="41" spans="1:4" ht="18.75">
       <c r="B41" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="C41" s="66" t="s">
+        <v>209</v>
+      </c>
+      <c r="D41" s="66" t="s">
         <v>210</v>
-      </c>
-      <c r="C41" s="66" t="s">
-        <v>212</v>
-      </c>
-      <c r="D41" s="66" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="117" customHeight="1">
       <c r="B42" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="C42" s="67" t="s">
         <v>211</v>
-      </c>
-      <c r="C42" s="67" t="s">
-        <v>214</v>
       </c>
       <c r="D42" s="58"/>
     </row>
@@ -4183,21 +4926,21 @@
     </row>
     <row r="44" spans="1:4" ht="18.75">
       <c r="B44" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="C44" s="56" t="s">
+        <v>238</v>
+      </c>
+      <c r="D44" s="66" t="s">
         <v>232</v>
-      </c>
-      <c r="C44" s="56" t="s">
-        <v>241</v>
-      </c>
-      <c r="D44" s="66" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="164.25" customHeight="1">
       <c r="B45" s="42" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C45" s="67" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D45" s="58"/>
     </row>
@@ -4206,21 +4949,21 @@
     </row>
     <row r="47" spans="1:4" ht="18.75">
       <c r="B47" s="40" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C47" s="56" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D47" s="56" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="120">
       <c r="B48" s="42" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C48" s="67" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D48" s="58"/>
     </row>
@@ -4275,100 +5018,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
-    <col min="3" max="3" width="119.7109375" customWidth="1"/>
-    <col min="4" max="4" width="148.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="25">
-        <v>1</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="29">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75">
-      <c r="B7" s="32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12">
-        <v>120</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4444,12 +5098,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5006,8 +5663,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:I505"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">

</xml_diff>